<commit_message>
thêm tình trạng của form chấm đeiẻm
</commit_message>
<xml_diff>
--- a/public/upload/student_list_each_semester/2/D14_TH03.xlsx
+++ b/public/upload/student_list_each_semester/2/D14_TH03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\danh gia ren luyen thay hung\danh-sach-sinh-vien-cntt 2018\CNTT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Laravel\luanvantotnghiep\public\upload\student_list_each_semester\2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -736,9 +736,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -755,6 +752,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -767,49 +809,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1095,7 +1095,7 @@
   <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F11" sqref="F11:O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1108,46 +1108,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="27" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
     </row>
     <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="37" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1156,76 +1156,76 @@
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
     </row>
     <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
     </row>
@@ -1247,52 +1247,52 @@
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="29" t="s">
+      <c r="D8" s="29"/>
+      <c r="E8" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="25" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="L8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="25" t="s">
+      <c r="M8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="25" t="s">
+      <c r="N8" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="25" t="s">
+      <c r="O8" s="26" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="31"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="30"/>
       <c r="F9" s="8" t="s">
         <v>20</v>
       </c>
@@ -1302,13 +1302,13 @@
       <c r="H9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
     </row>
     <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
@@ -1317,10 +1317,10 @@
       <c r="B10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="9" t="s">
         <v>26</v>
       </c>
@@ -1371,16 +1371,16 @@
       <c r="E11" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
@@ -1398,16 +1398,16 @@
       <c r="E12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
@@ -1425,16 +1425,16 @@
       <c r="E13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
@@ -1452,16 +1452,16 @@
       <c r="E14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
@@ -1479,16 +1479,16 @@
       <c r="E15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
@@ -1506,16 +1506,16 @@
       <c r="E16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
@@ -1533,16 +1533,16 @@
       <c r="E17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
@@ -1560,16 +1560,16 @@
       <c r="E18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
@@ -1587,16 +1587,16 @@
       <c r="E19" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
@@ -1614,16 +1614,16 @@
       <c r="E20" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
@@ -1641,16 +1641,16 @@
       <c r="E21" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
@@ -1668,16 +1668,16 @@
       <c r="E22" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
@@ -1695,16 +1695,16 @@
       <c r="E23" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
@@ -1722,16 +1722,16 @@
       <c r="E24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
@@ -1749,16 +1749,16 @@
       <c r="E25" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
@@ -1776,16 +1776,16 @@
       <c r="E26" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
@@ -1803,16 +1803,16 @@
       <c r="E27" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="39"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
@@ -1830,16 +1830,16 @@
       <c r="E28" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
@@ -1857,16 +1857,16 @@
       <c r="E29" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
@@ -1884,16 +1884,16 @@
       <c r="E30" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="39"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
@@ -1911,16 +1911,16 @@
       <c r="E31" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="39"/>
+      <c r="O31" s="39"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
@@ -1938,16 +1938,16 @@
       <c r="E32" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
@@ -1965,16 +1965,16 @@
       <c r="E33" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
+      <c r="O33" s="39"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="10">
@@ -1992,16 +1992,16 @@
       <c r="E34" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="39"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="10">
@@ -2019,16 +2019,16 @@
       <c r="E35" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="39"/>
+      <c r="O35" s="39"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
@@ -2046,16 +2046,16 @@
       <c r="E36" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="10">
@@ -2073,16 +2073,16 @@
       <c r="E37" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="39"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="10">
@@ -2100,16 +2100,16 @@
       <c r="E38" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="39"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
@@ -2127,16 +2127,16 @@
       <c r="E39" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="39"/>
+      <c r="O39" s="39"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="10">
@@ -2154,48 +2154,48 @@
       <c r="E40" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="39"/>
+      <c r="M40" s="39"/>
+      <c r="N40" s="39"/>
+      <c r="O40" s="39"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="16"/>
-      <c r="N41" s="16"/>
-      <c r="O41" s="16"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
     </row>
     <row r="42" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="23"/>
+      <c r="C42" s="37"/>
       <c r="D42" s="4"/>
       <c r="E42" s="7"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="24" t="s">
+      <c r="G42" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
       <c r="J42" s="4"/>
       <c r="K42" s="7"/>
       <c r="L42" s="7"/>
@@ -2207,18 +2207,18 @@
     </row>
     <row r="43" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="C43" s="23"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="4"/>
       <c r="E43" s="7"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="24" t="s">
+      <c r="G43" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
       <c r="J43" s="4"/>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
@@ -2231,8 +2231,8 @@
     <row r="44" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="7"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
@@ -2248,8 +2248,8 @@
     <row r="45" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="7"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
@@ -2265,8 +2265,8 @@
     <row r="46" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="7"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
@@ -2284,8 +2284,8 @@
         <v>126</v>
       </c>
       <c r="B47" s="7"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
@@ -2299,12 +2299,12 @@
       <c r="O47" s="7"/>
     </row>
     <row r="48" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="17" t="s">
         <v>127</v>
       </c>
       <c r="B48" s="7"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
@@ -2322,8 +2322,8 @@
         <v>128</v>
       </c>
       <c r="B49" s="7"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
@@ -2341,8 +2341,8 @@
         <v>129</v>
       </c>
       <c r="B50" s="7"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
@@ -2357,23 +2357,23 @@
     </row>
     <row r="51" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17" t="s">
+      <c r="C51" s="16"/>
+      <c r="D51" s="16" t="s">
         <v>131</v>
       </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
-      <c r="G51" s="20" t="s">
+      <c r="G51" s="19" t="s">
         <v>132</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
-      <c r="L51" s="19" t="s">
+      <c r="L51" s="18" t="s">
         <v>133</v>
       </c>
       <c r="M51" s="7"/>
@@ -2382,16 +2382,16 @@
     </row>
     <row r="52" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17" t="s">
+      <c r="C52" s="16"/>
+      <c r="D52" s="16" t="s">
         <v>135</v>
       </c>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
-      <c r="G52" s="20" t="s">
+      <c r="G52" s="19" t="s">
         <v>136</v>
       </c>
       <c r="H52" s="7"/>
@@ -2407,16 +2407,16 @@
     </row>
     <row r="53" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17" t="s">
+      <c r="C53" s="16"/>
+      <c r="D53" s="16" t="s">
         <v>139</v>
       </c>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
-      <c r="G53" s="20" t="s">
+      <c r="G53" s="19" t="s">
         <v>140</v>
       </c>
       <c r="H53" s="7"/>
@@ -2435,8 +2435,8 @@
         <v>142</v>
       </c>
       <c r="B54" s="7"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
@@ -2450,12 +2450,12 @@
       <c r="O54" s="7"/>
     </row>
     <row r="55" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="17" t="s">
         <v>143</v>
       </c>
       <c r="B55" s="7"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
@@ -2470,17 +2470,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:O1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:O2"/>
-    <mergeCell ref="G3:O3"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="G43:I43"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:M5"/>
@@ -2492,11 +2486,17 @@
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:O1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:O2"/>
+    <mergeCell ref="G3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>